<commit_message>
Refatoração tabela de sinais , adição da instrução CMP para o grupo R-type
</commit_message>
<xml_diff>
--- a/doc/architecture/Tabelas de Sinais.xlsx
+++ b/doc/architecture/Tabelas de Sinais.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="30">
   <si>
     <t>Tabelas de Sinais</t>
   </si>
   <si>
-    <t>ADD, SUB, MUL, DIV, AND, OR, NOT</t>
+    <t>ADD, SUB, MUL, DIV, AND, OR, NOT, CMP</t>
   </si>
   <si>
     <t>Estado 1</t>
@@ -77,7 +77,10 @@
     <t>write_pc</t>
   </si>
   <si>
-    <t>CMP</t>
+    <t>BRFL</t>
+  </si>
+  <si>
+    <t>FAZER AINDA</t>
   </si>
   <si>
     <t>ADDI, SUBI, ANDI, ORI</t>
@@ -118,6 +121,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,11 +143,13 @@
       <sz val="18"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -151,12 +157,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -377,10 +385,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F200"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A181" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F193" activeCellId="0" sqref="F193"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -781,8 +789,8 @@
       <c r="C26" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D26" s="6" t="n">
-        <v>1</v>
+      <c r="D26" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>0</v>
@@ -791,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -804,7 +812,7 @@
       <c r="D27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E27" s="7" t="n">
+      <c r="E27" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F27" s="2" t="n">
@@ -851,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
         <v>11</v>
       </c>
@@ -861,7 +869,7 @@
       <c r="C30" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D30" s="6" t="n">
+      <c r="D30" s="5" t="n">
         <v>0</v>
       </c>
       <c r="E30" s="5" t="n">
@@ -871,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -889,6 +897,9 @@
       </c>
       <c r="F31" s="8" t="n">
         <v>0</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
         <v>14</v>
       </c>
@@ -924,7 +935,7 @@
       <c r="D33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E33" s="7" t="n">
+      <c r="E33" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F33" s="2" t="n">
@@ -1011,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
         <v>19</v>
       </c>
@@ -1027,8 +1038,8 @@
       <c r="E38" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F38" s="6" t="n">
-        <v>1</v>
+      <c r="F38" s="5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,7 +1052,7 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1353,7 +1364,7 @@
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1665,7 +1676,7 @@
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1977,7 +1988,7 @@
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B94" s="12"/>
       <c r="C94" s="12"/>
@@ -2289,7 +2300,7 @@
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
@@ -2601,7 +2612,7 @@
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B130" s="12"/>
       <c r="C130" s="12"/>
@@ -2913,7 +2924,7 @@
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B148" s="12"/>
       <c r="C148" s="12"/>
@@ -3225,7 +3236,7 @@
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B166" s="12"/>
       <c r="C166" s="12"/>
@@ -3537,7 +3548,7 @@
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B184" s="12"/>
       <c r="C184" s="12"/>

</xml_diff>